<commit_message>
Added text files for Stats.py
</commit_message>
<xml_diff>
--- a/Result_data/KMeans_DE_SVM_10_6.xlsx
+++ b/Result_data/KMeans_DE_SVM_10_6.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Time" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$2:$I$306</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -361,15 +364,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E306"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A2:BS367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="K256" sqref="K256:BS256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -385,8 +389,20 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -403,7 +419,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -420,7 +436,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -437,7 +453,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -453,8 +469,20 @@
       <c r="E6">
         <v>400</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f>AVERAGE(B3:B6)</f>
+        <v>0.93375000000000008</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(C3:C6)</f>
+        <v>0.93399999999999994</v>
+      </c>
+      <c r="I6">
+        <f>AVERAGE(D3:D6)</f>
+        <v>0.93374999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -471,7 +499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -488,7 +516,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -505,7 +533,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -522,7 +550,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -538,8 +566,20 @@
       <c r="E11">
         <v>400</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f>AVERAGE(B8:B11)</f>
+        <v>0.93524999999999991</v>
+      </c>
+      <c r="H11">
+        <f>AVERAGE(C8:C11)</f>
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="I11">
+        <f>AVERAGE(D8:D11)</f>
+        <v>0.93550000000000011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -556,7 +596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -573,7 +613,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -590,7 +630,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -607,7 +647,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -623,8 +663,20 @@
       <c r="E16">
         <v>400</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f>AVERAGE(B13:B16)</f>
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H16">
+        <f>AVERAGE(C13:C16)</f>
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="I16">
+        <f>AVERAGE(D13:D16)</f>
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -641,7 +693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -658,7 +710,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -675,7 +727,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -692,7 +744,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -708,8 +760,20 @@
       <c r="E21">
         <v>400</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f>AVERAGE(B18:B21)</f>
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="H21">
+        <f>AVERAGE(C18:C21)</f>
+        <v>0.90574999999999994</v>
+      </c>
+      <c r="I21">
+        <f>AVERAGE(D18:D21)</f>
+        <v>0.90549999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -726,7 +790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -743,7 +807,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -760,7 +824,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -777,7 +841,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -793,8 +857,20 @@
       <c r="E26">
         <v>400</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f>AVERAGE(B23:B26)</f>
+        <v>0.92725000000000002</v>
+      </c>
+      <c r="H26">
+        <f>AVERAGE(C23:C26)</f>
+        <v>0.92725000000000002</v>
+      </c>
+      <c r="I26">
+        <f>AVERAGE(D23:D26)</f>
+        <v>0.92749999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -811,7 +887,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -828,7 +904,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -845,7 +921,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -862,7 +938,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4</v>
       </c>
@@ -878,8 +954,20 @@
       <c r="E31">
         <v>400</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <f>AVERAGE(B28:B31)</f>
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="H31">
+        <f>AVERAGE(C28:C31)</f>
+        <v>0.93474999999999997</v>
+      </c>
+      <c r="I31">
+        <f>AVERAGE(D28:D31)</f>
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -896,7 +984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -913,7 +1001,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -930,7 +1018,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -947,7 +1035,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -963,8 +1051,20 @@
       <c r="E36">
         <v>400</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f>AVERAGE(B33:B36)</f>
+        <v>0.9335</v>
+      </c>
+      <c r="H36">
+        <f>AVERAGE(C33:C36)</f>
+        <v>0.93375000000000008</v>
+      </c>
+      <c r="I36">
+        <f>AVERAGE(D33:D36)</f>
+        <v>0.93374999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -981,7 +1081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -998,7 +1098,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1015,7 +1115,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -1032,7 +1132,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1048,8 +1148,20 @@
       <c r="E41">
         <v>400</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <f>AVERAGE(B38:B41)</f>
+        <v>0.9285000000000001</v>
+      </c>
+      <c r="H41">
+        <f>AVERAGE(C38:C41)</f>
+        <v>0.92825000000000002</v>
+      </c>
+      <c r="I41">
+        <f>AVERAGE(D38:D41)</f>
+        <v>0.92849999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1083,7 +1195,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1100,7 +1212,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -1117,7 +1229,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -1133,8 +1245,20 @@
       <c r="E46">
         <v>400</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <f>AVERAGE(B43:B46)</f>
+        <v>0.9345</v>
+      </c>
+      <c r="H46">
+        <f>AVERAGE(C43:C46)</f>
+        <v>0.9345</v>
+      </c>
+      <c r="I46">
+        <f>AVERAGE(D43:D46)</f>
+        <v>0.93425000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -1168,7 +1292,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1185,7 +1309,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1202,7 +1326,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -1218,8 +1342,20 @@
       <c r="E51">
         <v>400</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <f>AVERAGE(B48:B51)</f>
+        <v>0.93125000000000013</v>
+      </c>
+      <c r="H51">
+        <f>AVERAGE(C48:C51)</f>
+        <v>0.93149999999999999</v>
+      </c>
+      <c r="I51">
+        <f>AVERAGE(D48:D51)</f>
+        <v>0.93124999999999991</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
@@ -1253,7 +1389,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -1270,7 +1406,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -1287,7 +1423,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4</v>
       </c>
@@ -1303,8 +1439,20 @@
       <c r="E56">
         <v>400</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <f>AVERAGE(B53:B56)</f>
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="H56">
+        <f>AVERAGE(C53:C56)</f>
+        <v>0.91874999999999996</v>
+      </c>
+      <c r="I56">
+        <f>AVERAGE(D53:D56)</f>
+        <v>0.9192499999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1</v>
       </c>
@@ -1338,7 +1486,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1355,7 +1503,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -1372,7 +1520,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -1388,8 +1536,20 @@
       <c r="E61">
         <v>400</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <f>AVERAGE(B58:B61)</f>
+        <v>0.93725000000000003</v>
+      </c>
+      <c r="H61">
+        <f>AVERAGE(C58:C61)</f>
+        <v>0.93725000000000003</v>
+      </c>
+      <c r="I61">
+        <f>AVERAGE(D58:D61)</f>
+        <v>0.93725000000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1</v>
       </c>
@@ -1423,7 +1583,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>
@@ -1440,7 +1600,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3</v>
       </c>
@@ -1457,7 +1617,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4</v>
       </c>
@@ -1473,8 +1633,20 @@
       <c r="E66">
         <v>400</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <f>AVERAGE(B63:B66)</f>
+        <v>0.94200000000000006</v>
+      </c>
+      <c r="H66">
+        <f>AVERAGE(C63:C66)</f>
+        <v>0.9415</v>
+      </c>
+      <c r="I66">
+        <f>AVERAGE(D63:D66)</f>
+        <v>0.94200000000000006</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -1491,7 +1663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1</v>
       </c>
@@ -1508,7 +1680,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2</v>
       </c>
@@ -1525,7 +1697,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3</v>
       </c>
@@ -1542,7 +1714,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>4</v>
       </c>
@@ -1558,8 +1730,20 @@
       <c r="E71">
         <v>400</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <f>AVERAGE(B68:B71)</f>
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="H71">
+        <f>AVERAGE(C68:C71)</f>
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="I71">
+        <f>AVERAGE(D68:D71)</f>
+        <v>0.91925000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -1576,7 +1760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1</v>
       </c>
@@ -1593,7 +1777,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2</v>
       </c>
@@ -1610,7 +1794,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3</v>
       </c>
@@ -1627,7 +1811,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4</v>
       </c>
@@ -1643,8 +1827,20 @@
       <c r="E76">
         <v>400</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <f>AVERAGE(B73:B76)</f>
+        <v>0.93550000000000011</v>
+      </c>
+      <c r="H76">
+        <f>AVERAGE(C73:C76)</f>
+        <v>0.9355</v>
+      </c>
+      <c r="I76">
+        <f>AVERAGE(D73:D76)</f>
+        <v>0.93550000000000011</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -1661,7 +1857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1</v>
       </c>
@@ -1678,7 +1874,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2</v>
       </c>
@@ -1695,7 +1891,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3</v>
       </c>
@@ -1712,7 +1908,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4</v>
       </c>
@@ -1728,8 +1924,20 @@
       <c r="E81">
         <v>400</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <f>AVERAGE(B78:B81)</f>
+        <v>0.93</v>
+      </c>
+      <c r="H81">
+        <f>AVERAGE(C78:C81)</f>
+        <v>0.93</v>
+      </c>
+      <c r="I81">
+        <f>AVERAGE(D78:D81)</f>
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -1746,7 +1954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1</v>
       </c>
@@ -1763,7 +1971,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2</v>
       </c>
@@ -1780,7 +1988,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>3</v>
       </c>
@@ -1797,7 +2005,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>4</v>
       </c>
@@ -1813,8 +2021,20 @@
       <c r="E86">
         <v>400</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G86">
+        <f>AVERAGE(B83:B86)</f>
+        <v>0.93575000000000008</v>
+      </c>
+      <c r="H86">
+        <f>AVERAGE(C83:C86)</f>
+        <v>0.93574999999999997</v>
+      </c>
+      <c r="I86">
+        <f>AVERAGE(D83:D86)</f>
+        <v>0.9355</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -1831,7 +2051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1</v>
       </c>
@@ -1848,7 +2068,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2</v>
       </c>
@@ -1865,7 +2085,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>3</v>
       </c>
@@ -1882,7 +2102,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>4</v>
       </c>
@@ -1898,8 +2118,20 @@
       <c r="E91">
         <v>400</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G91">
+        <f>AVERAGE(B88:B91)</f>
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="H91">
+        <f>AVERAGE(C88:C91)</f>
+        <v>0.92899999999999994</v>
+      </c>
+      <c r="I91">
+        <f>AVERAGE(D88:D91)</f>
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -1916,7 +2148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1</v>
       </c>
@@ -1933,7 +2165,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2</v>
       </c>
@@ -1950,7 +2182,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>3</v>
       </c>
@@ -1967,7 +2199,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>4</v>
       </c>
@@ -1983,8 +2215,20 @@
       <c r="E96">
         <v>400</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <f>AVERAGE(B93:B96)</f>
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="H96">
+        <f>AVERAGE(C93:C96)</f>
+        <v>0.9365</v>
+      </c>
+      <c r="I96">
+        <f>AVERAGE(D93:D96)</f>
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -2001,7 +2245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1</v>
       </c>
@@ -2018,7 +2262,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2</v>
       </c>
@@ -2035,7 +2279,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>3</v>
       </c>
@@ -2052,7 +2296,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>4</v>
       </c>
@@ -2068,8 +2312,20 @@
       <c r="E101">
         <v>400</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G101">
+        <f>AVERAGE(B98:B101)</f>
+        <v>0.92775000000000007</v>
+      </c>
+      <c r="H101">
+        <f>AVERAGE(C98:C101)</f>
+        <v>0.92825000000000002</v>
+      </c>
+      <c r="I101">
+        <f>AVERAGE(D98:D101)</f>
+        <v>0.92825000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -2086,7 +2342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1</v>
       </c>
@@ -2103,7 +2359,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2</v>
       </c>
@@ -2120,7 +2376,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>3</v>
       </c>
@@ -2137,7 +2393,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>4</v>
       </c>
@@ -2153,8 +2409,20 @@
       <c r="E106">
         <v>400</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G106">
+        <f>AVERAGE(B103:B106)</f>
+        <v>0.93274999999999997</v>
+      </c>
+      <c r="H106">
+        <f>AVERAGE(C103:C106)</f>
+        <v>0.93274999999999997</v>
+      </c>
+      <c r="I106">
+        <f>AVERAGE(D103:D106)</f>
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -2171,7 +2439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1</v>
       </c>
@@ -2188,7 +2456,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2</v>
       </c>
@@ -2205,7 +2473,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>3</v>
       </c>
@@ -2222,7 +2490,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>4</v>
       </c>
@@ -2238,8 +2506,20 @@
       <c r="E111">
         <v>400</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G111">
+        <f>AVERAGE(B108:B111)</f>
+        <v>0.92125000000000001</v>
+      </c>
+      <c r="H111">
+        <f>AVERAGE(C108:C111)</f>
+        <v>0.92075000000000007</v>
+      </c>
+      <c r="I111">
+        <f>AVERAGE(D108:D111)</f>
+        <v>0.92125000000000012</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>0</v>
       </c>
@@ -2256,7 +2536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1</v>
       </c>
@@ -2273,7 +2553,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2</v>
       </c>
@@ -2290,7 +2570,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>3</v>
       </c>
@@ -2307,7 +2587,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>4</v>
       </c>
@@ -2323,8 +2603,20 @@
       <c r="E116">
         <v>400</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G116">
+        <f>AVERAGE(B113:B116)</f>
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="H116">
+        <f>AVERAGE(C113:C116)</f>
+        <v>0.93074999999999997</v>
+      </c>
+      <c r="I116">
+        <f>AVERAGE(D113:D116)</f>
+        <v>0.93124999999999991</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -2341,7 +2633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1</v>
       </c>
@@ -2358,7 +2650,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2</v>
       </c>
@@ -2375,7 +2667,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>3</v>
       </c>
@@ -2392,7 +2684,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>4</v>
       </c>
@@ -2408,8 +2700,20 @@
       <c r="E121">
         <v>400</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G121">
+        <f>AVERAGE(B118:B121)</f>
+        <v>0.9395</v>
+      </c>
+      <c r="H121">
+        <f>AVERAGE(C118:C121)</f>
+        <v>0.93925000000000003</v>
+      </c>
+      <c r="I121">
+        <f>AVERAGE(D118:D121)</f>
+        <v>0.93899999999999995</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>0</v>
       </c>
@@ -2426,7 +2730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1</v>
       </c>
@@ -2443,7 +2747,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2</v>
       </c>
@@ -2460,7 +2764,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>3</v>
       </c>
@@ -2477,7 +2781,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>4</v>
       </c>
@@ -2493,8 +2797,20 @@
       <c r="E126">
         <v>400</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G126">
+        <f>AVERAGE(B123:B126)</f>
+        <v>0.92074999999999996</v>
+      </c>
+      <c r="H126">
+        <f>AVERAGE(C123:C126)</f>
+        <v>0.92074999999999996</v>
+      </c>
+      <c r="I126">
+        <f>AVERAGE(D123:D126)</f>
+        <v>0.92125000000000001</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -2511,7 +2827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1</v>
       </c>
@@ -2528,7 +2844,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2</v>
       </c>
@@ -2545,7 +2861,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>3</v>
       </c>
@@ -2562,7 +2878,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>4</v>
       </c>
@@ -2578,8 +2894,20 @@
       <c r="E131">
         <v>400</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G131">
+        <f>AVERAGE(B128:B131)</f>
+        <v>0.93699999999999994</v>
+      </c>
+      <c r="H131">
+        <f>AVERAGE(C128:C131)</f>
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="I131">
+        <f>AVERAGE(D128:D131)</f>
+        <v>0.93674999999999997</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>0</v>
       </c>
@@ -2596,7 +2924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>1</v>
       </c>
@@ -2613,7 +2941,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2</v>
       </c>
@@ -2630,7 +2958,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>3</v>
       </c>
@@ -2647,7 +2975,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>4</v>
       </c>
@@ -2663,8 +2991,20 @@
       <c r="E136">
         <v>400</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G136">
+        <f>AVERAGE(B133:B136)</f>
+        <v>0.9245000000000001</v>
+      </c>
+      <c r="H136">
+        <f>AVERAGE(C133:C136)</f>
+        <v>0.92475000000000007</v>
+      </c>
+      <c r="I136">
+        <f>AVERAGE(D133:D136)</f>
+        <v>0.92425000000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -2681,7 +3021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>1</v>
       </c>
@@ -2698,7 +3038,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2</v>
       </c>
@@ -2715,7 +3055,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>3</v>
       </c>
@@ -2732,7 +3072,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>4</v>
       </c>
@@ -2748,8 +3088,20 @@
       <c r="E141">
         <v>400</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G141">
+        <f>AVERAGE(B138:B141)</f>
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="H141">
+        <f>AVERAGE(C138:C141)</f>
+        <v>0.92225000000000001</v>
+      </c>
+      <c r="I141">
+        <f>AVERAGE(D138:D141)</f>
+        <v>0.92149999999999999</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>0</v>
       </c>
@@ -2766,7 +3118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1</v>
       </c>
@@ -2783,7 +3135,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2</v>
       </c>
@@ -2800,7 +3152,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>3</v>
       </c>
@@ -2817,7 +3169,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>4</v>
       </c>
@@ -2833,8 +3185,20 @@
       <c r="E146">
         <v>400</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G146">
+        <f>AVERAGE(B143:B146)</f>
+        <v>0.93025000000000002</v>
+      </c>
+      <c r="H146">
+        <f>AVERAGE(C143:C146)</f>
+        <v>0.93025000000000002</v>
+      </c>
+      <c r="I146">
+        <f>AVERAGE(D143:D146)</f>
+        <v>0.93049999999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -2851,7 +3215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1</v>
       </c>
@@ -2868,7 +3232,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2</v>
       </c>
@@ -2885,7 +3249,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>3</v>
       </c>
@@ -2902,7 +3266,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>4</v>
       </c>
@@ -2918,8 +3282,20 @@
       <c r="E151">
         <v>400</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G151">
+        <f>AVERAGE(B148:B151)</f>
+        <v>0.93525000000000003</v>
+      </c>
+      <c r="H151">
+        <f>AVERAGE(C148:C151)</f>
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="I151">
+        <f>AVERAGE(D148:D151)</f>
+        <v>0.9355</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -2936,7 +3312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1</v>
       </c>
@@ -2953,7 +3329,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2</v>
       </c>
@@ -2970,7 +3346,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>3</v>
       </c>
@@ -2987,7 +3363,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>4</v>
       </c>
@@ -3003,8 +3379,20 @@
       <c r="E156">
         <v>400</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G156">
+        <f>AVERAGE(B153:B156)</f>
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="H156">
+        <f>AVERAGE(C153:C156)</f>
+        <v>0.93425000000000014</v>
+      </c>
+      <c r="I156">
+        <f>AVERAGE(D153:D156)</f>
+        <v>0.93425000000000002</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>0</v>
       </c>
@@ -3021,7 +3409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1</v>
       </c>
@@ -3038,7 +3426,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2</v>
       </c>
@@ -3055,7 +3443,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>3</v>
       </c>
@@ -3072,7 +3460,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>4</v>
       </c>
@@ -3088,8 +3476,20 @@
       <c r="E161">
         <v>400</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G161">
+        <f>AVERAGE(B158:B161)</f>
+        <v>0.9285000000000001</v>
+      </c>
+      <c r="H161">
+        <f>AVERAGE(C158:C161)</f>
+        <v>0.92874999999999996</v>
+      </c>
+      <c r="I161">
+        <f>AVERAGE(D158:D161)</f>
+        <v>0.92849999999999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>0</v>
       </c>
@@ -3106,7 +3506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1</v>
       </c>
@@ -3123,7 +3523,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2</v>
       </c>
@@ -3140,7 +3540,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>3</v>
       </c>
@@ -3157,7 +3557,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>4</v>
       </c>
@@ -3173,8 +3573,20 @@
       <c r="E166">
         <v>400</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G166">
+        <f>AVERAGE(B163:B166)</f>
+        <v>0.93425000000000002</v>
+      </c>
+      <c r="H166">
+        <f>AVERAGE(C163:C166)</f>
+        <v>0.9345</v>
+      </c>
+      <c r="I166">
+        <f>AVERAGE(D163:D166)</f>
+        <v>0.93425000000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -3191,7 +3603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>1</v>
       </c>
@@ -3208,7 +3620,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2</v>
       </c>
@@ -3225,7 +3637,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>3</v>
       </c>
@@ -3242,7 +3654,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>4</v>
       </c>
@@ -3258,8 +3670,20 @@
       <c r="E171">
         <v>400</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G171">
+        <f>AVERAGE(B168:B171)</f>
+        <v>0.91475000000000006</v>
+      </c>
+      <c r="H171">
+        <f>AVERAGE(C168:C171)</f>
+        <v>0.91449999999999998</v>
+      </c>
+      <c r="I171">
+        <f>AVERAGE(D168:D171)</f>
+        <v>0.91475000000000006</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>0</v>
       </c>
@@ -3276,7 +3700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>1</v>
       </c>
@@ -3293,7 +3717,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2</v>
       </c>
@@ -3310,7 +3734,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>3</v>
       </c>
@@ -3327,7 +3751,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>4</v>
       </c>
@@ -3343,8 +3767,20 @@
       <c r="E176">
         <v>400</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G176">
+        <f>AVERAGE(B173:B176)</f>
+        <v>0.93975000000000009</v>
+      </c>
+      <c r="H176">
+        <f>AVERAGE(C173:C176)</f>
+        <v>0.94</v>
+      </c>
+      <c r="I176">
+        <f>AVERAGE(D173:D176)</f>
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>0</v>
       </c>
@@ -3361,7 +3797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1</v>
       </c>
@@ -3378,7 +3814,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2</v>
       </c>
@@ -3395,7 +3831,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>3</v>
       </c>
@@ -3412,7 +3848,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>4</v>
       </c>
@@ -3428,8 +3864,20 @@
       <c r="E181">
         <v>400</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G181">
+        <f>AVERAGE(B178:B181)</f>
+        <v>0.93025000000000002</v>
+      </c>
+      <c r="H181">
+        <f>AVERAGE(C178:C181)</f>
+        <v>0.93049999999999999</v>
+      </c>
+      <c r="I181">
+        <f>AVERAGE(D178:D181)</f>
+        <v>0.93049999999999999</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -3446,7 +3894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>1</v>
       </c>
@@ -3463,7 +3911,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>2</v>
       </c>
@@ -3480,7 +3928,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>3</v>
       </c>
@@ -3497,7 +3945,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>4</v>
       </c>
@@ -3513,8 +3961,20 @@
       <c r="E186">
         <v>400</v>
       </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G186">
+        <f>AVERAGE(B183:B186)</f>
+        <v>0.92549999999999999</v>
+      </c>
+      <c r="H186">
+        <f>AVERAGE(C183:C186)</f>
+        <v>0.92575000000000007</v>
+      </c>
+      <c r="I186">
+        <f>AVERAGE(D183:D186)</f>
+        <v>0.92574999999999996</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -3531,7 +3991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>1</v>
       </c>
@@ -3548,7 +4008,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>2</v>
       </c>
@@ -3565,7 +4025,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>3</v>
       </c>
@@ -3582,7 +4042,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>4</v>
       </c>
@@ -3598,8 +4058,20 @@
       <c r="E191">
         <v>400</v>
       </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G191">
+        <f>AVERAGE(B188:B191)</f>
+        <v>0.93175000000000008</v>
+      </c>
+      <c r="H191">
+        <f>AVERAGE(C188:C191)</f>
+        <v>0.93175000000000008</v>
+      </c>
+      <c r="I191">
+        <f>AVERAGE(D188:D191)</f>
+        <v>0.93174999999999997</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>0</v>
       </c>
@@ -3616,7 +4088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>1</v>
       </c>
@@ -3633,7 +4105,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>2</v>
       </c>
@@ -3650,7 +4122,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>3</v>
       </c>
@@ -3667,7 +4139,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>4</v>
       </c>
@@ -3683,8 +4155,20 @@
       <c r="E196">
         <v>400</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G196">
+        <f>AVERAGE(B193:B196)</f>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="H196">
+        <f>AVERAGE(C193:C196)</f>
+        <v>0.93199999999999994</v>
+      </c>
+      <c r="I196">
+        <f>AVERAGE(D193:D196)</f>
+        <v>0.93174999999999997</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>0</v>
       </c>
@@ -3701,7 +4185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>1</v>
       </c>
@@ -3718,7 +4202,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>2</v>
       </c>
@@ -3735,7 +4219,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>3</v>
       </c>
@@ -3752,7 +4236,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>4</v>
       </c>
@@ -3768,8 +4252,20 @@
       <c r="E201">
         <v>400</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G201">
+        <f>AVERAGE(B198:B201)</f>
+        <v>0.92249999999999999</v>
+      </c>
+      <c r="H201">
+        <f>AVERAGE(C198:C201)</f>
+        <v>0.92274999999999996</v>
+      </c>
+      <c r="I201">
+        <f>AVERAGE(D198:D201)</f>
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>0</v>
       </c>
@@ -3786,7 +4282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>1</v>
       </c>
@@ -3803,7 +4299,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>2</v>
       </c>
@@ -3820,7 +4316,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>3</v>
       </c>
@@ -3837,7 +4333,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>4</v>
       </c>
@@ -3853,8 +4349,20 @@
       <c r="E206">
         <v>400</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G206">
+        <f>AVERAGE(B203:B206)</f>
+        <v>0.92274999999999996</v>
+      </c>
+      <c r="H206">
+        <f>AVERAGE(C203:C206)</f>
+        <v>0.92274999999999996</v>
+      </c>
+      <c r="I206">
+        <f>AVERAGE(D203:D206)</f>
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>0</v>
       </c>
@@ -3871,7 +4379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>1</v>
       </c>
@@ -3888,7 +4396,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>2</v>
       </c>
@@ -3905,7 +4413,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>3</v>
       </c>
@@ -3922,7 +4430,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>4</v>
       </c>
@@ -3938,8 +4446,20 @@
       <c r="E211">
         <v>400</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G211">
+        <f>AVERAGE(B208:B211)</f>
+        <v>0.93875000000000008</v>
+      </c>
+      <c r="H211">
+        <f>AVERAGE(C208:C211)</f>
+        <v>0.93874999999999997</v>
+      </c>
+      <c r="I211">
+        <f>AVERAGE(D208:D211)</f>
+        <v>0.93850000000000011</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>0</v>
       </c>
@@ -3956,7 +4476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>1</v>
       </c>
@@ -3973,7 +4493,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>2</v>
       </c>
@@ -3990,7 +4510,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>3</v>
       </c>
@@ -4007,7 +4527,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>4</v>
       </c>
@@ -4023,8 +4543,20 @@
       <c r="E216">
         <v>400</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G216">
+        <f>AVERAGE(B213:B216)</f>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="H216">
+        <f>AVERAGE(C213:C216)</f>
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="I216">
+        <f>AVERAGE(D213:D216)</f>
+        <v>0.93175000000000008</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>0</v>
       </c>
@@ -4041,7 +4573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>1</v>
       </c>
@@ -4058,7 +4590,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>2</v>
       </c>
@@ -4075,7 +4607,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>3</v>
       </c>
@@ -4092,7 +4624,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>4</v>
       </c>
@@ -4108,8 +4640,20 @@
       <c r="E221">
         <v>400</v>
       </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G221">
+        <f>AVERAGE(B218:B221)</f>
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="H221">
+        <f>AVERAGE(C218:C221)</f>
+        <v>0.93399999999999994</v>
+      </c>
+      <c r="I221">
+        <f>AVERAGE(D218:D221)</f>
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>0</v>
       </c>
@@ -4126,7 +4670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>1</v>
       </c>
@@ -4143,7 +4687,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>2</v>
       </c>
@@ -4160,7 +4704,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>3</v>
       </c>
@@ -4177,7 +4721,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>4</v>
       </c>
@@ -4193,8 +4737,20 @@
       <c r="E226">
         <v>400</v>
       </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G226">
+        <f>AVERAGE(B223:B226)</f>
+        <v>0.93299999999999994</v>
+      </c>
+      <c r="H226">
+        <f>AVERAGE(C223:C226)</f>
+        <v>0.93274999999999997</v>
+      </c>
+      <c r="I226">
+        <f>AVERAGE(D223:D226)</f>
+        <v>0.93275000000000008</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>0</v>
       </c>
@@ -4211,7 +4767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>1</v>
       </c>
@@ -4228,7 +4784,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>2</v>
       </c>
@@ -4245,7 +4801,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>3</v>
       </c>
@@ -4262,7 +4818,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>4</v>
       </c>
@@ -4278,8 +4834,20 @@
       <c r="E231">
         <v>400</v>
       </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G231">
+        <f>AVERAGE(B228:B231)</f>
+        <v>0.91875000000000007</v>
+      </c>
+      <c r="H231">
+        <f>AVERAGE(C228:C231)</f>
+        <v>0.91875000000000007</v>
+      </c>
+      <c r="I231">
+        <f>AVERAGE(D228:D231)</f>
+        <v>0.91949999999999998</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>0</v>
       </c>
@@ -4296,7 +4864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>1</v>
       </c>
@@ -4313,7 +4881,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>2</v>
       </c>
@@ -4330,7 +4898,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>3</v>
       </c>
@@ -4347,7 +4915,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>4</v>
       </c>
@@ -4363,8 +4931,20 @@
       <c r="E236">
         <v>400</v>
       </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G236">
+        <f>AVERAGE(B233:B236)</f>
+        <v>0.94200000000000006</v>
+      </c>
+      <c r="H236">
+        <f>AVERAGE(C233:C236)</f>
+        <v>0.94175000000000009</v>
+      </c>
+      <c r="I236">
+        <f>AVERAGE(D233:D236)</f>
+        <v>0.94200000000000006</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>0</v>
       </c>
@@ -4381,7 +4961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>1</v>
       </c>
@@ -4398,7 +4978,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>2</v>
       </c>
@@ -4415,7 +4995,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>3</v>
       </c>
@@ -4432,7 +5012,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>4</v>
       </c>
@@ -4448,8 +5028,20 @@
       <c r="E241">
         <v>400</v>
       </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G241">
+        <f>AVERAGE(B238:B241)</f>
+        <v>0.92874999999999996</v>
+      </c>
+      <c r="H241">
+        <f>AVERAGE(C238:C241)</f>
+        <v>0.92899999999999994</v>
+      </c>
+      <c r="I241">
+        <f>AVERAGE(D238:D241)</f>
+        <v>0.9285000000000001</v>
+      </c>
+    </row>
+    <row r="242" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>0</v>
       </c>
@@ -4466,7 +5058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>1</v>
       </c>
@@ -4483,7 +5075,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>2</v>
       </c>
@@ -4500,7 +5092,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>3</v>
       </c>
@@ -4517,7 +5109,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>4</v>
       </c>
@@ -4533,8 +5125,20 @@
       <c r="E246">
         <v>400</v>
       </c>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G246">
+        <f>AVERAGE(B243:B246)</f>
+        <v>0.92325000000000013</v>
+      </c>
+      <c r="H246">
+        <f>AVERAGE(C243:C246)</f>
+        <v>0.9232499999999999</v>
+      </c>
+      <c r="I246">
+        <f>AVERAGE(D243:D246)</f>
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="247" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>0</v>
       </c>
@@ -4551,7 +5155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>1</v>
       </c>
@@ -4568,7 +5172,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>2</v>
       </c>
@@ -4585,7 +5189,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>3</v>
       </c>
@@ -4602,7 +5206,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>4</v>
       </c>
@@ -4618,8 +5222,20 @@
       <c r="E251">
         <v>400</v>
       </c>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G251">
+        <f>AVERAGE(B248:B251)</f>
+        <v>0.93550000000000011</v>
+      </c>
+      <c r="H251">
+        <f>AVERAGE(C248:C251)</f>
+        <v>0.93525000000000003</v>
+      </c>
+      <c r="I251">
+        <f>AVERAGE(D248:D251)</f>
+        <v>0.9355</v>
+      </c>
+    </row>
+    <row r="252" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>0</v>
       </c>
@@ -4636,7 +5252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>1</v>
       </c>
@@ -4653,7 +5269,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>2</v>
       </c>
@@ -4670,7 +5286,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:71" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>3</v>
       </c>
@@ -4687,7 +5303,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>4</v>
       </c>
@@ -4703,8 +5319,203 @@
       <c r="E256">
         <v>400</v>
       </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G256">
+        <f>AVERAGE(B253:B256)</f>
+        <v>0.9335</v>
+      </c>
+      <c r="H256">
+        <f>AVERAGE(C253:C256)</f>
+        <v>0.93375000000000008</v>
+      </c>
+      <c r="I256">
+        <f>AVERAGE(D253:D256)</f>
+        <v>0.93375000000000008</v>
+      </c>
+      <c r="K256">
+        <v>0.93374999999999997</v>
+      </c>
+      <c r="L256">
+        <v>0.93550000000000011</v>
+      </c>
+      <c r="M256">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="N256">
+        <v>0.90549999999999997</v>
+      </c>
+      <c r="O256">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="P256">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="Q256">
+        <v>0.93374999999999997</v>
+      </c>
+      <c r="R256">
+        <v>0.92849999999999999</v>
+      </c>
+      <c r="S256">
+        <v>0.93425000000000002</v>
+      </c>
+      <c r="T256">
+        <v>0.93124999999999991</v>
+      </c>
+      <c r="U256">
+        <v>0.9192499999999999</v>
+      </c>
+      <c r="V256">
+        <v>0.93725000000000003</v>
+      </c>
+      <c r="W256">
+        <v>0.94200000000000006</v>
+      </c>
+      <c r="X256">
+        <v>0.91925000000000001</v>
+      </c>
+      <c r="Y256">
+        <v>0.93550000000000011</v>
+      </c>
+      <c r="Z256">
+        <v>0.93</v>
+      </c>
+      <c r="AA256">
+        <v>0.9355</v>
+      </c>
+      <c r="AB256">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="AC256">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="AD256">
+        <v>0.92825000000000002</v>
+      </c>
+      <c r="AE256">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="AF256">
+        <v>0.92125000000000012</v>
+      </c>
+      <c r="AG256">
+        <v>0.93124999999999991</v>
+      </c>
+      <c r="AH256">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="AI256">
+        <v>0.92125000000000001</v>
+      </c>
+      <c r="AJ256">
+        <v>0.93674999999999997</v>
+      </c>
+      <c r="AK256">
+        <v>0.92425000000000002</v>
+      </c>
+      <c r="AL256">
+        <v>0.92149999999999999</v>
+      </c>
+      <c r="AM256">
+        <v>0.93049999999999999</v>
+      </c>
+      <c r="AN256">
+        <v>0.9355</v>
+      </c>
+      <c r="AO256">
+        <v>0.93425000000000002</v>
+      </c>
+      <c r="AP256">
+        <v>0.92849999999999999</v>
+      </c>
+      <c r="AQ256">
+        <v>0.93425000000000002</v>
+      </c>
+      <c r="AR256">
+        <v>0.91475000000000006</v>
+      </c>
+      <c r="AS256">
+        <v>0.94</v>
+      </c>
+      <c r="AT256">
+        <v>0.93049999999999999</v>
+      </c>
+      <c r="AU256">
+        <v>0.92574999999999996</v>
+      </c>
+      <c r="AV256">
+        <v>0.93174999999999997</v>
+      </c>
+      <c r="AW256">
+        <v>0.93174999999999997</v>
+      </c>
+      <c r="AX256">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="AY256">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="AZ256">
+        <v>0.93850000000000011</v>
+      </c>
+      <c r="BA256">
+        <v>0.93175000000000008</v>
+      </c>
+      <c r="BB256">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="BC256">
+        <v>0.93275000000000008</v>
+      </c>
+      <c r="BD256">
+        <v>0.91949999999999998</v>
+      </c>
+      <c r="BE256">
+        <v>0.94200000000000006</v>
+      </c>
+      <c r="BF256">
+        <v>0.9285000000000001</v>
+      </c>
+      <c r="BG256">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="BH256">
+        <v>0.9355</v>
+      </c>
+      <c r="BI256">
+        <v>0.93375000000000008</v>
+      </c>
+      <c r="BJ256">
+        <v>0.9385</v>
+      </c>
+      <c r="BK256">
+        <v>0.9355</v>
+      </c>
+      <c r="BL256">
+        <v>0.9225000000000001</v>
+      </c>
+      <c r="BM256">
+        <v>0.94249999999999989</v>
+      </c>
+      <c r="BN256">
+        <v>0.9305000000000001</v>
+      </c>
+      <c r="BO256">
+        <v>0.93874999999999997</v>
+      </c>
+      <c r="BP256">
+        <v>0.91649999999999998</v>
+      </c>
+      <c r="BQ256">
+        <v>0.9162499999999999</v>
+      </c>
+      <c r="BR256">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="BS256">
+        <v>0.9305000000000001</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>0</v>
       </c>
@@ -4721,7 +5532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>1</v>
       </c>
@@ -4738,7 +5549,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>2</v>
       </c>
@@ -4755,7 +5566,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>3</v>
       </c>
@@ -4772,7 +5583,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>4</v>
       </c>
@@ -4788,8 +5599,20 @@
       <c r="E261">
         <v>400</v>
       </c>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G261">
+        <f>AVERAGE(B258:B261)</f>
+        <v>0.93874999999999997</v>
+      </c>
+      <c r="H261">
+        <f>AVERAGE(C258:C261)</f>
+        <v>0.93900000000000006</v>
+      </c>
+      <c r="I261">
+        <f>AVERAGE(D258:D261)</f>
+        <v>0.9385</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>0</v>
       </c>
@@ -4806,7 +5629,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>1</v>
       </c>
@@ -4823,7 +5646,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>2</v>
       </c>
@@ -4840,7 +5663,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>3</v>
       </c>
@@ -4857,7 +5680,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>4</v>
       </c>
@@ -4873,8 +5696,20 @@
       <c r="E266">
         <v>400</v>
       </c>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G266">
+        <f>AVERAGE(B263:B266)</f>
+        <v>0.9355</v>
+      </c>
+      <c r="H266">
+        <f>AVERAGE(C263:C266)</f>
+        <v>0.93575000000000008</v>
+      </c>
+      <c r="I266">
+        <f>AVERAGE(D263:D266)</f>
+        <v>0.9355</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>0</v>
       </c>
@@ -4891,7 +5726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>1</v>
       </c>
@@ -4908,7 +5743,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>2</v>
       </c>
@@ -4925,7 +5760,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>3</v>
       </c>
@@ -4942,7 +5777,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>4</v>
       </c>
@@ -4958,8 +5793,20 @@
       <c r="E271">
         <v>400</v>
       </c>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G271">
+        <f>AVERAGE(B268:B271)</f>
+        <v>0.92225000000000001</v>
+      </c>
+      <c r="H271">
+        <f>AVERAGE(C268:C271)</f>
+        <v>0.92200000000000015</v>
+      </c>
+      <c r="I271">
+        <f>AVERAGE(D268:D271)</f>
+        <v>0.9225000000000001</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>0</v>
       </c>
@@ -4976,7 +5823,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>1</v>
       </c>
@@ -4993,7 +5840,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>2</v>
       </c>
@@ -5010,7 +5857,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>3</v>
       </c>
@@ -5027,7 +5874,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>4</v>
       </c>
@@ -5043,8 +5890,20 @@
       <c r="E276">
         <v>400</v>
       </c>
-    </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G276">
+        <f>AVERAGE(B273:B276)</f>
+        <v>0.9425</v>
+      </c>
+      <c r="H276">
+        <f>AVERAGE(C273:C276)</f>
+        <v>0.94275000000000009</v>
+      </c>
+      <c r="I276">
+        <f>AVERAGE(D273:D276)</f>
+        <v>0.94249999999999989</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>0</v>
       </c>
@@ -5061,7 +5920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>1</v>
       </c>
@@ -5078,7 +5937,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>2</v>
       </c>
@@ -5095,7 +5954,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>3</v>
       </c>
@@ -5112,7 +5971,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>4</v>
       </c>
@@ -5128,8 +5987,20 @@
       <c r="E281">
         <v>400</v>
       </c>
-    </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G281">
+        <f>AVERAGE(B278:B281)</f>
+        <v>0.93025000000000002</v>
+      </c>
+      <c r="H281">
+        <f>AVERAGE(C278:C281)</f>
+        <v>0.93025000000000002</v>
+      </c>
+      <c r="I281">
+        <f>AVERAGE(D278:D281)</f>
+        <v>0.9305000000000001</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>0</v>
       </c>
@@ -5146,7 +6017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>1</v>
       </c>
@@ -5163,7 +6034,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>2</v>
       </c>
@@ -5180,7 +6051,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>3</v>
       </c>
@@ -5197,7 +6068,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>4</v>
       </c>
@@ -5213,8 +6084,20 @@
       <c r="E286">
         <v>400</v>
       </c>
-    </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G286">
+        <f>AVERAGE(B283:B286)</f>
+        <v>0.93874999999999997</v>
+      </c>
+      <c r="H286">
+        <f>AVERAGE(C283:C286)</f>
+        <v>0.93900000000000006</v>
+      </c>
+      <c r="I286">
+        <f>AVERAGE(D283:D286)</f>
+        <v>0.93874999999999997</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>0</v>
       </c>
@@ -5231,7 +6114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1</v>
       </c>
@@ -5248,7 +6131,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>2</v>
       </c>
@@ -5265,7 +6148,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>3</v>
       </c>
@@ -5282,7 +6165,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>4</v>
       </c>
@@ -5298,8 +6181,20 @@
       <c r="E291">
         <v>400</v>
       </c>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G291">
+        <f>AVERAGE(B288:B291)</f>
+        <v>0.91675000000000006</v>
+      </c>
+      <c r="H291">
+        <f>AVERAGE(C288:C291)</f>
+        <v>0.91674999999999995</v>
+      </c>
+      <c r="I291">
+        <f>AVERAGE(D288:D291)</f>
+        <v>0.91649999999999998</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>0</v>
       </c>
@@ -5316,7 +6211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>1</v>
       </c>
@@ -5333,7 +6228,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>2</v>
       </c>
@@ -5350,7 +6245,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>3</v>
       </c>
@@ -5367,7 +6262,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>4</v>
       </c>
@@ -5383,8 +6278,20 @@
       <c r="E296">
         <v>400</v>
       </c>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G296">
+        <f>AVERAGE(B293:B296)</f>
+        <v>0.91625000000000001</v>
+      </c>
+      <c r="H296">
+        <f>AVERAGE(C293:C296)</f>
+        <v>0.9172499999999999</v>
+      </c>
+      <c r="I296">
+        <f>AVERAGE(D293:D296)</f>
+        <v>0.9162499999999999</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>0</v>
       </c>
@@ -5401,7 +6308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>1</v>
       </c>
@@ -5418,7 +6325,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>2</v>
       </c>
@@ -5435,7 +6342,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>3</v>
       </c>
@@ -5452,7 +6359,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>4</v>
       </c>
@@ -5468,8 +6375,20 @@
       <c r="E301">
         <v>400</v>
       </c>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G301">
+        <f>AVERAGE(B298:B301)</f>
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="H301">
+        <f>AVERAGE(C298:C301)</f>
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="I301">
+        <f>AVERAGE(D298:D301)</f>
+        <v>0.92749999999999999</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>0</v>
       </c>
@@ -5486,7 +6405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>1</v>
       </c>
@@ -5503,7 +6422,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>2</v>
       </c>
@@ -5520,7 +6439,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>3</v>
       </c>
@@ -5537,7 +6456,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>4</v>
       </c>
@@ -5553,8 +6472,332 @@
       <c r="E306">
         <v>24000</v>
       </c>
+      <c r="G306">
+        <f>AVERAGE(B303:B306)</f>
+        <v>0.93</v>
+      </c>
+      <c r="H306">
+        <f>AVERAGE(C303:C306)</f>
+        <v>0.92999999999999994</v>
+      </c>
+      <c r="I306">
+        <f>AVERAGE(D303:D306)</f>
+        <v>0.9305000000000001</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L307">
+        <v>0.93374999999999997</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L308">
+        <v>0.93550000000000011</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L309">
+        <v>0.93600000000000005</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L310">
+        <v>0.90549999999999997</v>
+      </c>
+    </row>
+    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L311">
+        <v>0.92749999999999999</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L312">
+        <v>0.93500000000000005</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L313">
+        <v>0.93374999999999997</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L314">
+        <v>0.92849999999999999</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L315">
+        <v>0.93425000000000002</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L316">
+        <v>0.93124999999999991</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L317">
+        <v>0.9192499999999999</v>
+      </c>
+    </row>
+    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L318">
+        <v>0.93725000000000003</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L319">
+        <v>0.94200000000000006</v>
+      </c>
+    </row>
+    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L320">
+        <v>0.91925000000000001</v>
+      </c>
+    </row>
+    <row r="321" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L321">
+        <v>0.93550000000000011</v>
+      </c>
+    </row>
+    <row r="322" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L322">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="323" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L323">
+        <v>0.9355</v>
+      </c>
+    </row>
+    <row r="324" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L324">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="325" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L325">
+        <v>0.93700000000000006</v>
+      </c>
+    </row>
+    <row r="326" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L326">
+        <v>0.92825000000000002</v>
+      </c>
+    </row>
+    <row r="327" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L327">
+        <v>0.93300000000000005</v>
+      </c>
+    </row>
+    <row r="328" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L328">
+        <v>0.92125000000000012</v>
+      </c>
+    </row>
+    <row r="329" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L329">
+        <v>0.93124999999999991</v>
+      </c>
+    </row>
+    <row r="330" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L330">
+        <v>0.93899999999999995</v>
+      </c>
+    </row>
+    <row r="331" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L331">
+        <v>0.92125000000000001</v>
+      </c>
+    </row>
+    <row r="332" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L332">
+        <v>0.93674999999999997</v>
+      </c>
+    </row>
+    <row r="333" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L333">
+        <v>0.92425000000000002</v>
+      </c>
+    </row>
+    <row r="334" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L334">
+        <v>0.92149999999999999</v>
+      </c>
+    </row>
+    <row r="335" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L335">
+        <v>0.93049999999999999</v>
+      </c>
+    </row>
+    <row r="336" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L336">
+        <v>0.9355</v>
+      </c>
+    </row>
+    <row r="337" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L337">
+        <v>0.93425000000000002</v>
+      </c>
+    </row>
+    <row r="338" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L338">
+        <v>0.92849999999999999</v>
+      </c>
+    </row>
+    <row r="339" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L339">
+        <v>0.93425000000000002</v>
+      </c>
+    </row>
+    <row r="340" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L340">
+        <v>0.91475000000000006</v>
+      </c>
+    </row>
+    <row r="341" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L341">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="342" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L342">
+        <v>0.93049999999999999</v>
+      </c>
+    </row>
+    <row r="343" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L343">
+        <v>0.92574999999999996</v>
+      </c>
+    </row>
+    <row r="344" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L344">
+        <v>0.93174999999999997</v>
+      </c>
+    </row>
+    <row r="345" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L345">
+        <v>0.93174999999999997</v>
+      </c>
+    </row>
+    <row r="346" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L346">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="347" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L347">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="348" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L348">
+        <v>0.93850000000000011</v>
+      </c>
+    </row>
+    <row r="349" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L349">
+        <v>0.93175000000000008</v>
+      </c>
+    </row>
+    <row r="350" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L350">
+        <v>0.93400000000000005</v>
+      </c>
+    </row>
+    <row r="351" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L351">
+        <v>0.93275000000000008</v>
+      </c>
+    </row>
+    <row r="352" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L352">
+        <v>0.91949999999999998</v>
+      </c>
+    </row>
+    <row r="353" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L353">
+        <v>0.94200000000000006</v>
+      </c>
+    </row>
+    <row r="354" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L354">
+        <v>0.9285000000000001</v>
+      </c>
+    </row>
+    <row r="355" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L355">
+        <v>0.92300000000000004</v>
+      </c>
+    </row>
+    <row r="356" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L356">
+        <v>0.9355</v>
+      </c>
+    </row>
+    <row r="357" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L357">
+        <v>0.93375000000000008</v>
+      </c>
+    </row>
+    <row r="358" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L358">
+        <v>0.9385</v>
+      </c>
+    </row>
+    <row r="359" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L359">
+        <v>0.9355</v>
+      </c>
+    </row>
+    <row r="360" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L360">
+        <v>0.9225000000000001</v>
+      </c>
+    </row>
+    <row r="361" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L361">
+        <v>0.94249999999999989</v>
+      </c>
+    </row>
+    <row r="362" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L362">
+        <v>0.9305000000000001</v>
+      </c>
+    </row>
+    <row r="363" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L363">
+        <v>0.93874999999999997</v>
+      </c>
+    </row>
+    <row r="364" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L364">
+        <v>0.91649999999999998</v>
+      </c>
+    </row>
+    <row r="365" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L365">
+        <v>0.9162499999999999</v>
+      </c>
+    </row>
+    <row r="366" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L366">
+        <v>0.92749999999999999</v>
+      </c>
+    </row>
+    <row r="367" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L367">
+        <v>0.9305000000000001</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:I306" xr:uid="{A1F4D1B4-ECC8-4CB3-A0D2-F9D115A56969}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="4"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5563,7 +6806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78D0768-2D92-46F6-A21D-DE3D97349D2E}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>